<commit_message>
add: add item of oa.nuist.edu.cn
</commit_message>
<xml_diff>
--- a/sonic-sheet.xlsx
+++ b/sonic-sheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="252">
   <si>
     <t>IP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1708,13 +1708,79 @@
   </si>
   <si>
     <t>实验室安全学习和考试系统</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>202.195.235.72</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oa.nuist.edu.cn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22, 80, 111, 8088, 8443, 9081</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(1)80:OA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>系统</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;(2)8088:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>泛微云桥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>e-Bridge;(3)9081:e-cology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>运维管理平台</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1800,7 +1866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1814,20 +1880,8 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1836,55 +1890,43 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1895,6 +1937,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1943,7 +1988,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1978,7 +2023,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2187,1477 +2232,1562 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E120"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10:C14"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="25.625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="50.625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="35.625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="25.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="4">
+      <c r="D2" s="12"/>
+      <c r="E2" s="13">
         <v>43279</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="25" t="s">
+      <c r="E3" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="25"/>
-      <c r="B5" s="5" t="s">
+      <c r="E4" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="25"/>
-      <c r="B6" s="5" t="s">
+      <c r="E5" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="11" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="25"/>
-      <c r="B7" s="5" t="s">
+      <c r="E6" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="11" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="25"/>
-      <c r="B8" s="5" t="s">
+      <c r="E7" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
+      <c r="E8" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="25" t="s">
+      <c r="E9" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="E10" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="25"/>
-      <c r="B11" s="5" t="s">
+      <c r="E10" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="25"/>
-      <c r="B12" s="5" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="25"/>
-      <c r="B13" s="5" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="25"/>
-      <c r="B14" s="5" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="19" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="12"/>
+      <c r="C15" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="13">
         <v>43279</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="13">
         <v>43278</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="13">
         <v>43261</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="12"/>
+      <c r="C18" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4">
+      <c r="D18" s="9"/>
+      <c r="E18" s="13">
         <v>43261</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4">
+      <c r="D19" s="9"/>
+      <c r="E19" s="13">
         <v>43261</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="12"/>
+      <c r="C20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4">
+      <c r="D20" s="9"/>
+      <c r="E20" s="13">
         <v>43261</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="12"/>
+      <c r="C21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4">
+      <c r="D21" s="9"/>
+      <c r="E21" s="13">
         <v>43261</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="12"/>
+      <c r="C22" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4">
+      <c r="D22" s="9"/>
+      <c r="E22" s="13">
         <v>43261</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="12"/>
+      <c r="C23" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4">
+      <c r="D23" s="9"/>
+      <c r="E23" s="13">
         <v>43261</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="12"/>
+      <c r="C24" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="13">
         <v>43261</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="B25" s="12"/>
+      <c r="C25" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="B26" s="12"/>
+      <c r="C26" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="3">
+      <c r="B28" s="12"/>
+      <c r="C28" s="9">
         <v>1521</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="4">
+      <c r="D28" s="9"/>
+      <c r="E28" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="B29" s="12"/>
+      <c r="C29" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="B31" s="12"/>
+      <c r="C31" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="B32" s="12"/>
+      <c r="C32" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="B33" s="12"/>
+      <c r="C33" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="4">
+      <c r="D33" s="9"/>
+      <c r="E33" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="B34" s="12"/>
+      <c r="C34" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="4">
+      <c r="D34" s="9"/>
+      <c r="E34" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:5" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="B36" s="12"/>
+      <c r="C36" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="B37" s="12"/>
+      <c r="C37" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="2" t="s">
+    <row r="38" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="B38" s="12"/>
+      <c r="C38" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="4">
+      <c r="D38" s="9"/>
+      <c r="E38" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="2" t="s">
+    <row r="39" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="B39" s="12"/>
+      <c r="C39" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="4">
+      <c r="D39" s="9"/>
+      <c r="E39" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="B40" s="12"/>
+      <c r="C40" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="4">
+      <c r="D40" s="9"/>
+      <c r="E40" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="2" t="s">
+    <row r="41" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="B41" s="12"/>
+      <c r="C41" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="4">
+      <c r="D41" s="9"/>
+      <c r="E41" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="2" t="s">
+    <row r="42" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="B42" s="12"/>
+      <c r="C42" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="4">
+      <c r="D42" s="9"/>
+      <c r="E42" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="2" t="s">
+    <row r="43" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="B43" s="12"/>
+      <c r="C43" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="4">
+      <c r="D43" s="9"/>
+      <c r="E43" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="2" t="s">
+    <row r="44" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="B44" s="12"/>
+      <c r="C44" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="4">
+      <c r="D44" s="9"/>
+      <c r="E44" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="2" t="s">
+    <row r="45" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="B45" s="12"/>
+      <c r="C45" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="2" t="s">
+    <row r="46" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="B46" s="12"/>
+      <c r="C46" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46" s="13">
         <v>43262</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="2" t="s">
+    <row r="47" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="B47" s="12"/>
+      <c r="C47" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E47" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="2" t="s">
+      <c r="E47" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="B48" s="12"/>
+      <c r="C48" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="E48" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="2" t="s">
+      <c r="E48" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="B49" s="12"/>
+      <c r="C49" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E49" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="2" t="s">
+      <c r="E49" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="B50" s="12"/>
+      <c r="C50" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E50" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="2" t="s">
+      <c r="E50" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="B51" s="12"/>
+      <c r="C51" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E51" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="2" t="s">
+      <c r="E51" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="B52" s="12"/>
+      <c r="C52" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E52" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="2" t="s">
+      <c r="E52" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="B53" s="12"/>
+      <c r="C53" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E53" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="2" t="s">
+      <c r="E53" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="B54" s="12"/>
+      <c r="C54" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E54" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="2" t="s">
+      <c r="E54" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="B55" s="12"/>
+      <c r="C55" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E55" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="2" t="s">
+      <c r="E55" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="B56" s="12"/>
+      <c r="C56" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E56" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="2" t="s">
+      <c r="E56" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="B57" s="12"/>
+      <c r="C57" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E57" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="2" t="s">
+      <c r="E57" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="B58" s="12"/>
+      <c r="C58" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E58" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="2" t="s">
+      <c r="E58" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="B59" s="12"/>
+      <c r="C59" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E59" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="2" t="s">
+      <c r="E59" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="B60" s="12"/>
+      <c r="C60" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E60" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="2" t="s">
+      <c r="E60" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="B61" s="12"/>
+      <c r="C61" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E61" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="2" t="s">
+      <c r="E61" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="B62" s="12"/>
+      <c r="C62" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="E62" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="2" t="s">
+      <c r="E62" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="B63" s="12"/>
+      <c r="C63" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="E63" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="2" t="s">
+      <c r="E63" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="B64" s="12"/>
+      <c r="C64" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D64" s="7"/>
-      <c r="E64" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="2" t="s">
+      <c r="D64" s="9"/>
+      <c r="E64" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="B65" s="12"/>
+      <c r="C65" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D65" s="7"/>
-      <c r="E65" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="2" t="s">
+      <c r="D65" s="9"/>
+      <c r="E65" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="C66" s="7">
+      <c r="B66" s="12"/>
+      <c r="C66" s="9">
         <v>22</v>
       </c>
-      <c r="D66" s="7"/>
-      <c r="E66" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="2" t="s">
+      <c r="D66" s="9"/>
+      <c r="E66" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="B67" s="12"/>
+      <c r="C67" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D67" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="E67" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="2" t="s">
+      <c r="E67" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="B68" s="12"/>
+      <c r="C68" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E68" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="2" t="s">
+      <c r="E68" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="B69" s="12"/>
+      <c r="C69" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="E69" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="2" t="s">
+      <c r="E69" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="B70" s="12"/>
+      <c r="C70" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="E70" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="2" t="s">
+      <c r="E70" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="B71" s="12"/>
+      <c r="C71" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D71" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="E71" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="2" t="s">
+      <c r="E71" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="B72" s="12"/>
+      <c r="C72" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="E72" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="2" t="s">
+      <c r="E72" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="C73" s="7" t="s">
+      <c r="B73" s="12"/>
+      <c r="C73" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E73" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="2" t="s">
+      <c r="E73" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="B74" s="12"/>
+      <c r="C74" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D74" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="E74" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="2" t="s">
+      <c r="E74" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="C75" s="7" t="s">
+      <c r="B75" s="12"/>
+      <c r="C75" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="D75" s="7" t="s">
+      <c r="D75" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E75" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="2" t="s">
+      <c r="E75" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="B76" s="12"/>
+      <c r="C76" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D76" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="E76" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="2" t="s">
+      <c r="E76" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="B77" s="12"/>
+      <c r="C77" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E77" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="2" t="s">
+      <c r="E77" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="B78" s="12"/>
+      <c r="C78" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="D78" s="7" t="s">
+      <c r="D78" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="E78" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="2" t="s">
+      <c r="E78" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="B79" s="12"/>
+      <c r="C79" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D79" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="E79" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="2" t="s">
+      <c r="E79" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="B80" s="12"/>
+      <c r="C80" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D80" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="E80" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="2" t="s">
+      <c r="E80" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="C81" s="7" t="s">
+      <c r="B81" s="12"/>
+      <c r="C81" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="D81" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="E81" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="2" t="s">
+      <c r="E81" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="C82" s="7" t="s">
+      <c r="B82" s="12"/>
+      <c r="C82" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="D82" s="7" t="s">
+      <c r="D82" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="E82" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="2" t="s">
+      <c r="E82" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="C83" s="7">
+      <c r="B83" s="12"/>
+      <c r="C83" s="9">
         <v>22</v>
       </c>
-      <c r="D83" s="7"/>
-      <c r="E83" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="2" t="s">
+      <c r="D83" s="9"/>
+      <c r="E83" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C84" s="7">
+      <c r="B84" s="12"/>
+      <c r="C84" s="9">
         <v>8080</v>
       </c>
-      <c r="D84" s="7"/>
-      <c r="E84" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="2" t="s">
+      <c r="D84" s="9"/>
+      <c r="E84" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="B85" s="12"/>
+      <c r="C85" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="D85" s="7"/>
-      <c r="E85" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="2" t="s">
+      <c r="D85" s="9"/>
+      <c r="E85" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="B86" s="12"/>
+      <c r="C86" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="D86" s="7"/>
-      <c r="E86" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="8" t="s">
+      <c r="D86" s="9"/>
+      <c r="E86" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="C87" s="12" t="s">
+      <c r="C87" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="D87" s="13" t="s">
+      <c r="D87" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="E87" s="4">
+      <c r="E87" s="13">
         <v>43278</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="2" t="s">
+    <row r="88" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B88" s="10" t="s">
+      <c r="B88" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C88" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D88" s="13" t="s">
+      <c r="D88" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="E88" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="2" t="s">
+      <c r="E88" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B89" s="9"/>
-      <c r="C89" s="7" t="s">
+      <c r="B89" s="14"/>
+      <c r="C89" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="D89" s="13" t="s">
+      <c r="D89" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="E89" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="25" t="s">
+      <c r="E89" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B90" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="E90" s="13">
+        <v>43426</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B91" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C90" s="26" t="s">
+      <c r="C91" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D90" s="13" t="s">
+      <c r="D91" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="E90" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="25"/>
-      <c r="B91" s="5" t="s">
+      <c r="E91" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="15"/>
+      <c r="B92" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C91" s="26"/>
-      <c r="D91" s="13" t="s">
+      <c r="C92" s="11"/>
+      <c r="D92" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="E91" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="25"/>
-      <c r="B92" s="5" t="s">
+      <c r="E92" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="15"/>
+      <c r="B93" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C92" s="26"/>
-      <c r="D92" s="13" t="s">
+      <c r="C93" s="11"/>
+      <c r="D93" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E92" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="25"/>
-      <c r="B93" s="5" t="s">
+      <c r="E93" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="15"/>
+      <c r="B94" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C93" s="26"/>
-      <c r="D93" s="21" t="s">
+      <c r="C94" s="11"/>
+      <c r="D94" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="E93" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="25" t="s">
+      <c r="E94" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="B94" s="27" t="s">
+      <c r="B95" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="C94" s="23">
+      <c r="C95" s="9">
         <v>80</v>
       </c>
-      <c r="D94" s="22" t="s">
+      <c r="D95" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="E94" s="4">
+      <c r="E95" s="13">
         <v>43424</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="25"/>
-      <c r="B95" s="27"/>
-      <c r="C95" s="23">
+    <row r="96" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="15"/>
+      <c r="B96" s="20"/>
+      <c r="C96" s="9">
         <v>8080</v>
       </c>
-      <c r="D95" s="11" t="s">
+      <c r="D96" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="E95" s="4">
+      <c r="E96" s="13">
         <v>43424</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B96" s="10" t="s">
+      <c r="B97" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C96" s="7" t="s">
+      <c r="C97" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D96" s="21" t="s">
+      <c r="D97" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="E96" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="14" t="s">
+      <c r="E97" s="13">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B98" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="C97" s="15" t="s">
+      <c r="C98" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="D97" s="21" t="s">
+      <c r="D98" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="E97" s="4">
+      <c r="E98" s="13">
         <v>43278</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="2" t="s">
+    <row r="99" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B99" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C99" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D98" s="21" t="s">
+      <c r="D99" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="E98" s="4">
+      <c r="E99" s="13">
         <v>43261</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="2" t="s">
+    <row r="100" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B100" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="C99" s="3">
+      <c r="C100" s="9">
         <v>80</v>
       </c>
-      <c r="D99" s="21" t="s">
+      <c r="D100" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="E99" s="4">
+      <c r="E100" s="13">
         <v>43390</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D100" s="21"/>
-    </row>
-    <row r="101" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D101" s="21"/>
-    </row>
-    <row r="102" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="28" t="s">
+    <row r="101" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D101" s="8"/>
+    </row>
+    <row r="102" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D102" s="8"/>
+    </row>
+    <row r="103" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="D102" s="7"/>
-    </row>
-    <row r="103" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="2" t="s">
+      <c r="D103" s="5"/>
+    </row>
+    <row r="104" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B104" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D103" s="7" t="s">
+      <c r="D104" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E103" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B104" s="10" t="s">
+      <c r="E104" s="4">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="D104" s="3"/>
-      <c r="E104" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B105" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="D105" s="3"/>
       <c r="E105" s="4">
         <v>43267</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="2" t="s">
+    <row r="106" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D106" s="3"/>
+      <c r="E106" s="4">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B107" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D106" s="11" t="s">
+      <c r="D107" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E106" s="4">
-        <v>43267</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B107" s="10" t="s">
+      <c r="E107" s="4">
+        <v>43267</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="6" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="109" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="110" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="111" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="112" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="113" ht="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="114" ht="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="115" ht="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="116" ht="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="117" ht="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="118" ht="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="119" ht="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="120" ht="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="109" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="C91:C94"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="B95:B96"/>
     <mergeCell ref="C10:C14"/>
     <mergeCell ref="C4:C8"/>
     <mergeCell ref="A4:A8"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="C90:C93"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>